<commit_message>
Updated Supplementary Tables (some modifications in column names, and adjusted for stretches spanning multiple genes
</commit_message>
<xml_diff>
--- a/Supplementary_files/Supplementary_Table_02.xlsx
+++ b/Supplementary_files/Supplementary_Table_02.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iamakhilverma/Desktop/SARS_CoV_2_region_conservation/Supplementary_files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54731A0C-60F8-F144-AE0A-BBB026605345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Mutations in &gt;= 100 NTs stretch" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -97,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,14 +155,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -215,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,27 +233,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -299,24 +267,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -492,18 +442,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="128.83203125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -519,7 +465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -527,7 +473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -535,7 +481,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -543,7 +489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -551,7 +497,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -559,7 +505,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -567,7 +513,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -575,7 +521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -583,7 +529,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -591,7 +537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added latest versions for Supplementary files
</commit_message>
<xml_diff>
--- a/Supplementary_files/Supplementary_Table_02.xlsx
+++ b/Supplementary_files/Supplementary_Table_02.xlsx
@@ -55,37 +55,37 @@
     <t>Conserved stretch 11</t>
   </si>
   <si>
+    <t>T973C, C1009T, G1006T, G942A, A949G, C958T, A1045T, G960A, G1043A, C952T</t>
+  </si>
+  <si>
+    <t>C8407T, C8480T, T8473C, A8456G, G8488A, C8481T, C8476T, C8502T, A8413G</t>
+  </si>
+  <si>
     <t>G12191T, C12295T, G12202T, C12312T, C12171T, C12325T, C12242T, G12223T, C12213T, G12223A, G12188T, G12163T, A12173G, C12241T, G12163A, G12243A</t>
   </si>
   <si>
+    <t>T12628C, T12640C, C12559T, G12565T, A12644G, C12624A, A12544G, C12616T, A12634G, C12623T, G12569A</t>
+  </si>
+  <si>
+    <t>C13424T, C13366T, C13426T, C13432T, C13372T, C13384T, C13436T, C13452T, C13378T, C13381T, C13424A, C13446T, C13423T, C13405T, C13421T</t>
+  </si>
+  <si>
+    <t>G16795T, A16797G, C16767T, C16806T, C16762T, G16827A, G16846T, T16800C, C16751A</t>
+  </si>
+  <si>
+    <t>T17865C, A17858G, G17944T, C17934T, C17862T, A17853T, T17963C, C17883T, G17893T, C17913T, A17916G</t>
+  </si>
+  <si>
+    <t>C19512T, C19488T, C19402T, G19518T, A19476G, G19419A, A19515G, T19519C, C19495T, T19521C, G19509T, G19509A, G19480T, T19452A, T19404C</t>
+  </si>
+  <si>
     <t>T24224C, G24257T, C24319T, A24253T, C24237T, G24328T, C24223T, G24236T, G24332T</t>
   </si>
   <si>
-    <t>C19512T, C19488T, C19402T, G19518T, A19476G, G19419A, A19515G, T19519C, C19495T, T19521C, G19509T, G19509A, G19480T, T19452A, T19404C</t>
-  </si>
-  <si>
-    <t>C8407T, C8480T, T8473C, A8456G, G8488A, C8481T, C8476T, C8502T, A8413G</t>
-  </si>
-  <si>
-    <t>T12628C, T12640C, C12559T, G12565T, A12644G, C12624A, A12544G, C12616T, A12634G, C12623T, G12569A</t>
-  </si>
-  <si>
-    <t>T17865C, A17858G, G17944T, C17934T, C17862T, A17853T, T17963C, C17883T, G17893T, C17913T, A17916G</t>
-  </si>
-  <si>
-    <t>T973C, C1009T, G1006T, G942A, A949G, C958T, A1045T, G960A, G1043A, C952T</t>
+    <t>C24700T, G24697A, A24673G, C24707A, T24733C, T24739C, C24715T, T24703C</t>
   </si>
   <si>
     <t>C26408T, A26319G, C26340T, A26358G, G26389T, C26366T, G26314A, G26325A</t>
-  </si>
-  <si>
-    <t>C24700T, G24697A, A24673G, C24707A, T24733C, T24739C, C24715T, T24703C</t>
-  </si>
-  <si>
-    <t>G16795T, A16797G, C16767T, C16806T, C16762T, G16827A, G16846T, T16800C, C16751A</t>
-  </si>
-  <si>
-    <t>C13424T, C13366T, C13426T, C13432T, C13372T, C13384T, C13436T, C13452T, C13378T, C13381T, C13424A, C13446T, C13423T, C13405T, C13421T</t>
   </si>
 </sst>
 </file>

</xml_diff>